<commit_message>
Update IT2 Dark Room xlsx file with room measures
</commit_message>
<xml_diff>
--- a/calibration/Physical Setup Measures/IT2 Black Room - Setup B.xlsx
+++ b/calibration/Physical Setup Measures/IT2 Black Room - Setup B.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25095" windowHeight="12600"/>
+    <workbookView windowWidth="25095" windowHeight="12600" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Setup Height" sheetId="2" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Velodyne" sheetId="4" r:id="rId3"/>
     <sheet name="Hesai Height" sheetId="1" r:id="rId4"/>
     <sheet name="Hesai Position" sheetId="5" r:id="rId5"/>
+    <sheet name="Room Dimensions" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -137,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="80">
   <si>
     <t>LiDAR and Camera Experimental Setup</t>
   </si>
@@ -365,6 +366,18 @@
   </si>
   <si>
     <t>B4</t>
+  </si>
+  <si>
+    <t>Room Dimensions</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
   </si>
 </sst>
 </file>
@@ -372,17 +385,26 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="178" formatCode="0.000_ "/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0.000_ "/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="24">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -413,15 +435,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -438,9 +451,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -454,45 +489,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -514,23 +521,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,15 +537,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -561,6 +553,27 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -575,13 +588,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,19 +642,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,13 +672,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,49 +684,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -695,7 +702,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,13 +738,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,37 +768,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -869,6 +882,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -883,11 +911,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -918,21 +952,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -942,17 +961,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -961,130 +974,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1093,10 +1106,10 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1106,68 +1119,65 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1179,9 +1189,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1221,28 +1228,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1251,7 +1258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1575,7 +1582,7 @@
   <sheetPr/>
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="I15" sqref="I15"/>
@@ -1613,7 +1620,7 @@
       <c r="V1" s="10"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:22">
-      <c r="A2" s="35"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1629,16 +1636,16 @@
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1651,592 +1658,592 @@
       <c r="V2" s="11"/>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:22">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="47" t="s">
+      <c r="M3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="N3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="O3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="47" t="s">
+      <c r="P3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="Q3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="R3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="47" t="s">
+      <c r="S3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="46" t="s">
+      <c r="T3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="46" t="s">
+      <c r="U3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="47" t="s">
+      <c r="V3" s="45" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:22">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="37">
         <v>0</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="37">
         <v>0</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="37">
         <v>0</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="37">
         <v>0.829</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="37">
         <v>0.829</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="37">
         <v>0.829</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="37">
         <v>0.842</v>
       </c>
-      <c r="I4" s="39">
+      <c r="I4" s="37">
         <v>0.842</v>
       </c>
-      <c r="J4" s="39">
+      <c r="J4" s="37">
         <v>0.842</v>
       </c>
-      <c r="K4" s="39">
+      <c r="K4" s="37">
         <f t="shared" ref="K4:M4" si="0">K$6+H4</f>
         <v>0.916</v>
       </c>
-      <c r="L4" s="39">
+      <c r="L4" s="37">
         <f t="shared" si="0"/>
         <v>0.917</v>
       </c>
-      <c r="M4" s="39">
+      <c r="M4" s="37">
         <f t="shared" si="0"/>
         <v>0.917</v>
       </c>
-      <c r="N4" s="48">
+      <c r="N4" s="46">
         <f t="shared" ref="N4:P4" si="1">N$7+K4</f>
         <v>0.91745</v>
       </c>
-      <c r="O4" s="48">
+      <c r="O4" s="46">
         <f t="shared" si="1"/>
         <v>0.91845</v>
       </c>
-      <c r="P4" s="48">
+      <c r="P4" s="46">
         <f t="shared" si="1"/>
         <v>0.91845</v>
       </c>
-      <c r="Q4" s="39">
+      <c r="Q4" s="37">
         <f t="shared" ref="Q4:S4" si="2">Q$6+E4</f>
         <v>0.93</v>
       </c>
-      <c r="R4" s="39">
+      <c r="R4" s="37">
         <f t="shared" si="2"/>
         <v>0.93</v>
       </c>
-      <c r="S4" s="39">
+      <c r="S4" s="37">
         <f t="shared" si="2"/>
         <v>0.93</v>
       </c>
-      <c r="T4" s="48">
+      <c r="T4" s="46">
         <f t="shared" ref="T4:V4" si="3">T$9+Q4</f>
         <v>0.9677</v>
       </c>
-      <c r="U4" s="48">
+      <c r="U4" s="46">
         <f t="shared" si="3"/>
         <v>0.9677</v>
       </c>
-      <c r="V4" s="48">
+      <c r="V4" s="46">
         <f t="shared" si="3"/>
         <v>0.9677</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:22">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="39">
+      <c r="B5" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="37">
         <v>0</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="37">
         <v>0</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="37">
         <v>0</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="37">
         <f t="shared" ref="H5:J5" si="4">H4-E4</f>
         <v>0.013</v>
       </c>
-      <c r="I5" s="39">
+      <c r="I5" s="37">
         <f t="shared" si="4"/>
         <v>0.013</v>
       </c>
-      <c r="J5" s="39">
+      <c r="J5" s="37">
         <f t="shared" si="4"/>
         <v>0.013</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="37">
         <f t="shared" ref="K5:M5" si="5">K$6+H5</f>
         <v>0.087</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="37">
         <f t="shared" si="5"/>
         <v>0.088</v>
       </c>
-      <c r="M5" s="39">
+      <c r="M5" s="37">
         <f t="shared" si="5"/>
         <v>0.088</v>
       </c>
-      <c r="N5" s="48">
+      <c r="N5" s="46">
         <f t="shared" ref="N5:P5" si="6">N$7+K5</f>
         <v>0.08845</v>
       </c>
-      <c r="O5" s="48">
+      <c r="O5" s="46">
         <f t="shared" si="6"/>
         <v>0.08945</v>
       </c>
-      <c r="P5" s="48">
+      <c r="P5" s="46">
         <f t="shared" si="6"/>
         <v>0.08945</v>
       </c>
-      <c r="Q5" s="39">
+      <c r="Q5" s="37">
         <f t="shared" ref="Q5:S5" si="7">Q$6+H5</f>
         <v>0.114</v>
       </c>
-      <c r="R5" s="39">
+      <c r="R5" s="37">
         <f t="shared" si="7"/>
         <v>0.114</v>
       </c>
-      <c r="S5" s="39">
+      <c r="S5" s="37">
         <f t="shared" si="7"/>
         <v>0.114</v>
       </c>
-      <c r="T5" s="48">
+      <c r="T5" s="46">
         <f t="shared" ref="T5:V5" si="8">T$9+Q5</f>
         <v>0.1517</v>
       </c>
-      <c r="U5" s="48">
+      <c r="U5" s="46">
         <f t="shared" si="8"/>
         <v>0.1517</v>
       </c>
-      <c r="V5" s="48">
+      <c r="V5" s="46">
         <f t="shared" si="8"/>
         <v>0.1517</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:22">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="39">
+      <c r="B6" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="37">
         <v>0</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="37">
         <v>0</v>
       </c>
-      <c r="J6" s="39">
+      <c r="J6" s="37">
         <v>0</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="37">
         <v>0.074</v>
       </c>
-      <c r="L6" s="39">
+      <c r="L6" s="37">
         <v>0.075</v>
       </c>
-      <c r="M6" s="39">
+      <c r="M6" s="37">
         <v>0.075</v>
       </c>
-      <c r="N6" s="48">
+      <c r="N6" s="46">
         <f t="shared" ref="N6:P6" si="9">N$7+K6</f>
         <v>0.07545</v>
       </c>
-      <c r="O6" s="48">
+      <c r="O6" s="46">
         <f t="shared" si="9"/>
         <v>0.07645</v>
       </c>
-      <c r="P6" s="48">
+      <c r="P6" s="46">
         <f t="shared" si="9"/>
         <v>0.07645</v>
       </c>
-      <c r="Q6" s="39">
+      <c r="Q6" s="37">
         <v>0.101</v>
       </c>
-      <c r="R6" s="39">
+      <c r="R6" s="37">
         <v>0.101</v>
       </c>
-      <c r="S6" s="39">
+      <c r="S6" s="37">
         <v>0.101</v>
       </c>
-      <c r="T6" s="48">
+      <c r="T6" s="46">
         <f t="shared" ref="T6:V6" si="10">T$9+Q6</f>
         <v>0.1387</v>
       </c>
-      <c r="U6" s="48">
+      <c r="U6" s="46">
         <f t="shared" si="10"/>
         <v>0.1387</v>
       </c>
-      <c r="V6" s="48">
+      <c r="V6" s="46">
         <f t="shared" si="10"/>
         <v>0.1387</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:22">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="39">
+      <c r="B7" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="37">
         <v>0</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="37">
         <v>0</v>
       </c>
-      <c r="M7" s="39">
+      <c r="M7" s="37">
         <v>0</v>
       </c>
-      <c r="N7" s="48">
+      <c r="N7" s="46">
         <f t="shared" ref="N7:P7" si="11">0.0029/2</f>
         <v>0.00145</v>
       </c>
-      <c r="O7" s="48">
+      <c r="O7" s="46">
         <f t="shared" si="11"/>
         <v>0.00145</v>
       </c>
-      <c r="P7" s="48">
+      <c r="P7" s="46">
         <f t="shared" si="11"/>
         <v>0.00145</v>
       </c>
-      <c r="Q7" s="39">
+      <c r="Q7" s="37">
         <f t="shared" ref="Q7:S7" si="12">Q$6-K6</f>
         <v>0.027</v>
       </c>
-      <c r="R7" s="39">
+      <c r="R7" s="37">
         <f t="shared" si="12"/>
         <v>0.026</v>
       </c>
-      <c r="S7" s="39">
+      <c r="S7" s="37">
         <f t="shared" si="12"/>
         <v>0.026</v>
       </c>
-      <c r="T7" s="48">
+      <c r="T7" s="46">
         <f t="shared" ref="T7:V7" si="13">T$9+Q7</f>
         <v>0.0647</v>
       </c>
-      <c r="U7" s="48">
+      <c r="U7" s="46">
         <f t="shared" si="13"/>
         <v>0.0637</v>
       </c>
-      <c r="V7" s="48">
+      <c r="V7" s="46">
         <f t="shared" si="13"/>
         <v>0.0637</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:22">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="39">
+      <c r="B8" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="37">
         <v>0</v>
       </c>
-      <c r="O8" s="39">
+      <c r="O8" s="37">
         <v>0</v>
       </c>
-      <c r="P8" s="39">
+      <c r="P8" s="37">
         <v>0</v>
       </c>
-      <c r="Q8" s="48">
+      <c r="Q8" s="46">
         <f t="shared" ref="Q8:S8" si="14">Q$6-N6</f>
         <v>0.02555</v>
       </c>
-      <c r="R8" s="48">
+      <c r="R8" s="46">
         <f t="shared" si="14"/>
         <v>0.02455</v>
       </c>
-      <c r="S8" s="48">
+      <c r="S8" s="46">
         <f t="shared" si="14"/>
         <v>0.02455</v>
       </c>
-      <c r="T8" s="48">
+      <c r="T8" s="46">
         <f t="shared" ref="T8:V8" si="15">T$9+Q8</f>
         <v>0.06325</v>
       </c>
-      <c r="U8" s="48">
+      <c r="U8" s="46">
         <f t="shared" si="15"/>
         <v>0.06225</v>
       </c>
-      <c r="V8" s="48">
+      <c r="V8" s="46">
         <f t="shared" si="15"/>
         <v>0.06225</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:22">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q9" s="39">
+      <c r="B9" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="37">
         <v>0</v>
       </c>
-      <c r="R9" s="39">
+      <c r="R9" s="37">
         <v>0</v>
       </c>
-      <c r="S9" s="39">
+      <c r="S9" s="37">
         <v>0</v>
       </c>
-      <c r="T9" s="48">
+      <c r="T9" s="46">
         <v>0.0377</v>
       </c>
-      <c r="U9" s="48">
+      <c r="U9" s="46">
         <v>0.0377</v>
       </c>
-      <c r="V9" s="48">
+      <c r="V9" s="46">
         <v>0.0377</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:22">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="P10" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="R10" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="S10" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="T10" s="39">
+      <c r="B10" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="R10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="37">
         <v>0</v>
       </c>
-      <c r="U10" s="39">
+      <c r="U10" s="37">
         <v>0</v>
       </c>
-      <c r="V10" s="39">
+      <c r="V10" s="37">
         <v>0</v>
       </c>
     </row>
@@ -2290,285 +2297,285 @@
       <c r="J1" s="10"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:10">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="20">
         <v>16</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="22"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:10">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="E3" s="34" t="s">
+      <c r="C3" s="25"/>
+      <c r="E3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="34" t="s">
+      <c r="G3" s="21"/>
+      <c r="H3" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="22"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:10">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>2.33</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="E4" s="34" t="s">
+      <c r="C4" s="25"/>
+      <c r="E4" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="34" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="22"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:10">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="E5" s="34" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="E5" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="34" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="22"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:10">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>3.216</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="H6" s="34" t="s">
+      <c r="C6" s="25"/>
+      <c r="H6" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="30">
         <v>1.49</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:10">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>1.608</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="E7" s="34" t="s">
+      <c r="C7" s="25"/>
+      <c r="E7" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="30">
         <v>1</v>
       </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="32" t="s">
+      <c r="H7" s="32"/>
+      <c r="I7" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="30">
         <v>2.36</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:10">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>1.3522</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="E8" s="34" t="s">
+      <c r="C8" s="25"/>
+      <c r="E8" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="30">
         <v>1</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="22"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:6">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>8.4153</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="E9" s="34" t="s">
+      <c r="C9" s="25"/>
+      <c r="E9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:6">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>7.0632</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="34" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:6">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <v>0.9778</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="27">
         <v>0.1384</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="34" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:6">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>6.0853</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="27">
         <v>0.8616</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="25"/>
+      <c r="E12" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1" spans="4:7">
-      <c r="D13" s="27"/>
-      <c r="E13" s="34" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="30">
         <v>0</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" ht="30" customHeight="1" spans="1:7">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>1.379</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="34" t="s">
+      <c r="D14" s="25"/>
+      <c r="E14" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="30">
         <v>2056</v>
       </c>
-      <c r="G14" s="22"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" ht="30" customHeight="1" spans="1:7">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="28">
         <v>2.334</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="34" t="s">
+      <c r="D15" s="25"/>
+      <c r="E15" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="30">
         <v>2452</v>
       </c>
-      <c r="G15" s="22"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" ht="30" customHeight="1" spans="4:7">
-      <c r="D16" s="27"/>
-      <c r="G16" s="22"/>
+      <c r="D16" s="25"/>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" ht="30" customHeight="1" spans="4:7">
-      <c r="D17" s="27"/>
-      <c r="G17" s="22"/>
+      <c r="D17" s="25"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" ht="30" customHeight="1" spans="7:7">
-      <c r="G18" s="22"/>
+      <c r="G18" s="21"/>
     </row>
     <row r="19" ht="30" customHeight="1" spans="7:7">
-      <c r="G19" s="22"/>
+      <c r="G19" s="21"/>
     </row>
     <row r="20" ht="30" customHeight="1" spans="7:7">
-      <c r="G20" s="22"/>
+      <c r="G20" s="21"/>
     </row>
     <row r="21" ht="30" customHeight="1" spans="7:7">
-      <c r="G21" s="22"/>
+      <c r="G21" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2587,45 +2594,45 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" ht="49" customHeight="1" spans="1:11">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>6.04</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1.799</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <f>'Setup Height'!V4</f>
         <v>0.9677</v>
       </c>
@@ -2682,7 +2689,7 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
-      <c r="K1" s="19"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" ht="51" customHeight="1" spans="2:22">
       <c r="B2" s="11" t="s">
@@ -2701,25 +2708,25 @@
       <c r="G2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="22"/>
+      <c r="V2" s="21"/>
     </row>
     <row r="3" ht="19" customHeight="1" spans="1:22">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <f>'Setup Height'!V4-D4</f>
         <v>0.9122</v>
       </c>
@@ -2727,96 +2734,96 @@
       <c r="F3" s="17">
         <v>0.85</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <f>D$3*F3</f>
         <v>0.77537</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <f>ROUND(G3,3)</f>
         <v>0.775</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="20">
         <f>'Setup Height'!V$4-(H3+D$4)</f>
         <v>0.1372</v>
       </c>
-      <c r="V3" s="22"/>
+      <c r="V3" s="21"/>
     </row>
     <row r="4" ht="19" customHeight="1" spans="1:22">
       <c r="A4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.0555</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17">
         <v>1</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>D$3*F4</f>
         <v>0.9122</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="7">
         <f>ROUND(G4,3)</f>
         <v>0.912</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="20">
         <f>'Setup Height'!V$4-(H4+D$4)</f>
         <v>0.000199999999999867</v>
       </c>
-      <c r="V4" s="23"/>
+      <c r="V4" s="22"/>
     </row>
     <row r="5" ht="19" customHeight="1" spans="1:22">
       <c r="A5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="17">
         <v>1.15</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f>D$3*F5</f>
         <v>1.04903</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <f>ROUND(G5,3)</f>
         <v>1.049</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="20">
         <f>'Setup Height'!V$4-(H5+D$4)</f>
         <v>-0.1368</v>
       </c>
-      <c r="V5" s="23"/>
+      <c r="V5" s="22"/>
     </row>
     <row r="6" ht="19" customHeight="1" spans="22:22">
-      <c r="V6" s="23"/>
+      <c r="V6" s="22"/>
     </row>
     <row r="7" ht="19" customHeight="1" spans="22:22">
-      <c r="V7" s="23"/>
+      <c r="V7" s="22"/>
     </row>
     <row r="8" ht="19" customHeight="1" spans="22:22">
-      <c r="V8" s="23"/>
+      <c r="V8" s="22"/>
     </row>
     <row r="9" ht="19" customHeight="1" spans="22:22">
-      <c r="V9" s="23"/>
+      <c r="V9" s="22"/>
     </row>
     <row r="10" ht="19" customHeight="1" spans="22:22">
-      <c r="V10" s="23"/>
+      <c r="V10" s="22"/>
     </row>
     <row r="11" spans="16:21">
       <c r="P11" s="9"/>
@@ -2832,12 +2839,12 @@
       <c r="U12" s="9"/>
     </row>
     <row r="17" customFormat="1" ht="33" customHeight="1" spans="12:12">
-      <c r="L17" s="19"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" ht="57" customHeight="1"/>
     <row r="19" ht="29" customHeight="1"/>
-    <row r="20" customFormat="1" ht="27" customHeight="1"/>
-    <row r="21" customFormat="1" ht="31" customHeight="1"/>
+    <row r="20" ht="27" customHeight="1"/>
+    <row r="21" ht="31" customHeight="1"/>
     <row r="22" customFormat="1" ht="27" customHeight="1" spans="1:10">
       <c r="A22" s="13"/>
       <c r="B22" s="9"/>
@@ -2862,17 +2869,17 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" customFormat="1" ht="33" customHeight="1"/>
-    <row r="25" customFormat="1" ht="32" customHeight="1"/>
-    <row r="26" customFormat="1" ht="32" customHeight="1"/>
-    <row r="27" customFormat="1" ht="30" customHeight="1"/>
-    <row r="28" customFormat="1" ht="41" customHeight="1"/>
-    <row r="29" customFormat="1" ht="30" customHeight="1"/>
-    <row r="30" customFormat="1" ht="30" customHeight="1"/>
-    <row r="31" customFormat="1" ht="30" customHeight="1"/>
-    <row r="32" customFormat="1" ht="30" customHeight="1"/>
-    <row r="33" customFormat="1" ht="30" customHeight="1"/>
-    <row r="34" customFormat="1" ht="30" customHeight="1"/>
+    <row r="24" ht="33" customHeight="1"/>
+    <row r="25" ht="32" customHeight="1"/>
+    <row r="26" ht="32" customHeight="1"/>
+    <row r="27" ht="30" customHeight="1"/>
+    <row r="28" ht="41" customHeight="1"/>
+    <row r="29" ht="30" customHeight="1"/>
+    <row r="30" ht="30" customHeight="1"/>
+    <row r="31" ht="30" customHeight="1"/>
+    <row r="32" ht="30" customHeight="1"/>
+    <row r="33" ht="30" customHeight="1"/>
+    <row r="34" ht="30" customHeight="1"/>
     <row r="35" ht="30" customHeight="1"/>
     <row r="36" ht="30" customHeight="1"/>
     <row r="37" ht="30" customHeight="1"/>
@@ -2884,12 +2891,12 @@
       <c r="A40" s="14"/>
     </row>
     <row r="46" ht="24" spans="7:12">
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2903,325 +2910,325 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" ht="53" customHeight="1" spans="3:9">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="G1" s="7" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="G1" s="8" t="s">
         <v>68</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="3:9">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:9">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>4.497</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1.793</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.765</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <f>Velodyne!A$3-C3</f>
         <v>1.543</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <f>D3-Velodyne!B$3</f>
         <v>-0.00600000000000001</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <f>(E3+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>-0.1472</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:9">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>4.497</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>1.783</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.902</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>Velodyne!A$3-C4</f>
         <v>1.543</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <f>D4-Velodyne!B$3</f>
         <v>-0.016</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <f>(E4+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>-0.0101999999999999</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:9">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>4.497</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1.788</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1.047</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f>Velodyne!A$3-C5</f>
         <v>1.543</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <f>D5-Velodyne!B$3</f>
         <v>-0.0109999999999999</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <f>(E5+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>0.1348</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:9">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>3.016</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>1.861</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.765</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f>Velodyne!A$3-C6</f>
         <v>3.024</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <f>D6-Velodyne!B$3</f>
         <v>0.0620000000000001</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <f>(E6+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>-0.1472</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:9">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>3.016</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>1.868</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.902</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f>Velodyne!A$3-C7</f>
         <v>3.024</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <f>D7-Velodyne!B$3</f>
         <v>0.0690000000000002</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <f>(E7+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>-0.0101999999999999</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:9">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>3.016</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>1.849</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>1.047</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f>Velodyne!A$3-C8</f>
         <v>3.024</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <f>D8-Velodyne!B$3</f>
         <v>0.05</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <f>(E8+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>0.1348</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>1.5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1.821</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>0.765</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f>Velodyne!A$3-C9</f>
         <v>4.54</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <f>D9-Velodyne!B$3</f>
         <v>0.022</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <f>(E9+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>-0.1472</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:9">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>1.5</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>1.827</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>0.902</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <f>Velodyne!A$3-C10</f>
         <v>4.54</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <f>D10-Velodyne!B$3</f>
         <v>0.028</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <f>(E10+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>-0.0101999999999999</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:9">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>1.5</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>1.821</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>1.047</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <f>Velodyne!A$3-C11</f>
         <v>4.54</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <f>D11-Velodyne!B$3</f>
         <v>0.022</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <f>(E11+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>0.1348</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:9">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6">
+      <c r="B12" s="2"/>
+      <c r="C12" s="7">
         <v>1.5</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>4.418</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>1.26</v>
       </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <f>Velodyne!A$3-C12</f>
         <v>4.54</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <f>D12-Velodyne!B$3</f>
         <v>2.619</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <f>(E12+'Hesai Height'!D$4)-'Setup Height'!V$4</f>
         <v>0.3478</v>
       </c>
@@ -3238,4 +3245,62 @@
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" ht="49" customHeight="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:3">
+      <c r="A3" s="2">
+        <v>5.196</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6.973</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.802</v>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>